<commit_message>
Error en la creación de usuarios
</commit_message>
<xml_diff>
--- a/CSVs/schema.xlsx
+++ b/CSVs/schema.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\apiSQLite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\panel\apiSQLite\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D694D4DF-E23A-42D2-874B-488B1B87881D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C039A5AC-B77F-4ABB-BF10-7B8E2023AB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
+    <sheet name="consulate" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">consulate!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="118">
   <si>
     <t>table</t>
   </si>
@@ -219,6 +223,174 @@
   </si>
   <si>
     <t>Nombre</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>about sections</t>
+  </si>
+  <si>
+    <t>collaborators?</t>
+  </si>
+  <si>
+    <t>collaborators type</t>
+  </si>
+  <si>
+    <t>editors</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>work type</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>agency</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>director</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>vimeo</t>
+  </si>
+  <si>
+    <t>youtube</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>tik tok</t>
+  </si>
+  <si>
+    <t>pinterest</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>contact_type</t>
+  </si>
+  <si>
+    <t>home_image</t>
+  </si>
+  <si>
+    <t>home_text</t>
+  </si>
+  <si>
+    <t>main_image</t>
+  </si>
+  <si>
+    <t>has_collaborator_list</t>
+  </si>
+  <si>
+    <t>main_video</t>
+  </si>
+  <si>
+    <t>bio_picture</t>
+  </si>
+  <si>
+    <t>show_home</t>
+  </si>
+  <si>
+    <t>order_home</t>
+  </si>
+  <si>
+    <t>short_video</t>
+  </si>
+  <si>
+    <t>complete_video</t>
+  </si>
+  <si>
+    <t>show_slide_home</t>
+  </si>
+  <si>
+    <t>order_slide_home</t>
+  </si>
+  <si>
+    <t>html_editor</t>
+  </si>
+  <si>
+    <t>related_link</t>
+  </si>
+  <si>
+    <t>related_news</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>work_type_1_to_many</t>
+  </si>
+  <si>
+    <t>work_type_1_to_1</t>
+  </si>
+  <si>
+    <t>referencia</t>
+  </si>
+  <si>
+    <t>consulate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -784,6 +956,29 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3E6D400C-AE9B-4A94-9510-AF9648A0BBDD}" name="Table4" displayName="Table4" ref="A1:N147" totalsRowShown="0">
+  <autoFilter ref="A1:N147" xr:uid="{3E6D400C-AE9B-4A94-9510-AF9648A0BBDD}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{50240153-99E2-46C1-9246-4A8F7C5C9919}" name=" "/>
+    <tableColumn id="2" xr3:uid="{AD517DB3-31A6-402B-BEB2-8A79379DEDBD}" name="table"/>
+    <tableColumn id="3" xr3:uid="{33991726-9D89-4E6B-AFA5-AF94CC7536A2}" name="column"/>
+    <tableColumn id="4" xr3:uid="{0FAE633D-2C58-4BFF-AFAD-2C0806ED0658}" name="displayName"/>
+    <tableColumn id="5" xr3:uid="{CFE79E9B-DDB4-4326-A6B6-563C0481193D}" name="isNullable"/>
+    <tableColumn id="6" xr3:uid="{7383DD47-BF56-4494-A8EC-3A521054EB91}" name="showInList"/>
+    <tableColumn id="7" xr3:uid="{17F025AD-284C-433D-8D86-8125E359DBE0}" name="dataType"/>
+    <tableColumn id="8" xr3:uid="{FD3B1A9B-ECF1-420A-97F5-A6BCEF545BDB}" name="length"/>
+    <tableColumn id="9" xr3:uid="{54BB885D-D195-42E4-9558-70B02C04E5DB}" name="position"/>
+    <tableColumn id="10" xr3:uid="{925AA276-520B-43E0-9586-A5344341CC31}" name="dafaultValue"/>
+    <tableColumn id="11" xr3:uid="{194E5510-3DD3-4BAA-9ADF-CC553DC852A6}" name="relationTable"/>
+    <tableColumn id="12" xr3:uid="{4DC87F11-2158-49C5-B64C-AC9F2A5EE616}" name="relationType"/>
+    <tableColumn id="13" xr3:uid="{9FA796AA-0D3A-4E34-A246-615AE04BB2F5}" name="link"/>
+    <tableColumn id="14" xr3:uid="{9B1B1B58-A243-49AA-AAFF-0EB7D4832B20}" name="columnInForm"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1083,7 +1278,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2784,4 +2981,3448 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A8F800-B5B3-4BF4-9830-541887FC217E}">
+  <dimension ref="A1:S147"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="S6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="S7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="S9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>200</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="S10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11">
+        <v>200</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="S11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>200</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19">
+        <v>200</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>200</v>
+      </c>
+      <c r="I20">
+        <v>8</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22">
+        <v>200</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="N26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27">
+        <v>200</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28">
+        <v>200</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30">
+        <v>200</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+      <c r="I34">
+        <v>6</v>
+      </c>
+      <c r="N34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35">
+        <v>200</v>
+      </c>
+      <c r="I35">
+        <v>7</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36">
+        <v>200</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="N36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38">
+        <v>200</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="N41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42">
+        <v>200</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
+      </c>
+      <c r="N42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43">
+        <v>200</v>
+      </c>
+      <c r="I43">
+        <v>7</v>
+      </c>
+      <c r="N43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44">
+        <v>10</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45">
+        <v>200</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46">
+        <v>200</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="K46" t="s">
+        <v>24</v>
+      </c>
+      <c r="L46" t="s">
+        <v>21</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>4</v>
+      </c>
+      <c r="K47" t="s">
+        <v>53</v>
+      </c>
+      <c r="L47" t="s">
+        <v>21</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48">
+        <v>6</v>
+      </c>
+      <c r="N48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49">
+        <v>10</v>
+      </c>
+      <c r="I49">
+        <v>9</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50">
+        <v>10</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>19</v>
+      </c>
+      <c r="H51">
+        <v>200</v>
+      </c>
+      <c r="I51">
+        <v>11</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52">
+        <v>200</v>
+      </c>
+      <c r="I52">
+        <v>12</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53">
+        <v>10</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54">
+        <v>200</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56">
+        <v>10</v>
+      </c>
+      <c r="I56">
+        <v>4</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57">
+        <v>200</v>
+      </c>
+      <c r="I57">
+        <v>5</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58">
+        <v>200</v>
+      </c>
+      <c r="I58">
+        <v>6</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" t="s">
+        <v>96</v>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>116</v>
+      </c>
+      <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>116</v>
+      </c>
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>71</v>
+      </c>
+      <c r="D68" t="s">
+        <v>71</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" t="s">
+        <v>73</v>
+      </c>
+      <c r="D69" t="s">
+        <v>73</v>
+      </c>
+      <c r="I69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" t="s">
+        <v>77</v>
+      </c>
+      <c r="I70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" t="s">
+        <v>74</v>
+      </c>
+      <c r="I71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" t="s">
+        <v>78</v>
+      </c>
+      <c r="D72" t="s">
+        <v>78</v>
+      </c>
+      <c r="I72">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" t="s">
+        <v>99</v>
+      </c>
+      <c r="I73">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" t="s">
+        <v>20</v>
+      </c>
+      <c r="I75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" t="s">
+        <v>111</v>
+      </c>
+      <c r="D77" t="s">
+        <v>111</v>
+      </c>
+      <c r="I77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>116</v>
+      </c>
+      <c r="B78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" t="s">
+        <v>72</v>
+      </c>
+      <c r="I78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>116</v>
+      </c>
+      <c r="B79" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" t="s">
+        <v>74</v>
+      </c>
+      <c r="D79" t="s">
+        <v>74</v>
+      </c>
+      <c r="I79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" t="s">
+        <v>78</v>
+      </c>
+      <c r="I80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>116</v>
+      </c>
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" t="s">
+        <v>18</v>
+      </c>
+      <c r="I81">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>116</v>
+      </c>
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="I82">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>116</v>
+      </c>
+      <c r="B83" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>116</v>
+      </c>
+      <c r="B84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84" t="s">
+        <v>72</v>
+      </c>
+      <c r="D84" t="s">
+        <v>72</v>
+      </c>
+      <c r="I84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85" t="s">
+        <v>65</v>
+      </c>
+      <c r="C85" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" t="s">
+        <v>74</v>
+      </c>
+      <c r="I85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>116</v>
+      </c>
+      <c r="B86" t="s">
+        <v>65</v>
+      </c>
+      <c r="C86" t="s">
+        <v>112</v>
+      </c>
+      <c r="D86" t="s">
+        <v>112</v>
+      </c>
+      <c r="I86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>116</v>
+      </c>
+      <c r="B87" t="s">
+        <v>65</v>
+      </c>
+      <c r="C87" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" t="s">
+        <v>18</v>
+      </c>
+      <c r="I87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B88" t="s">
+        <v>65</v>
+      </c>
+      <c r="C88" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" t="s">
+        <v>20</v>
+      </c>
+      <c r="I88">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C90" t="s">
+        <v>72</v>
+      </c>
+      <c r="D90" t="s">
+        <v>72</v>
+      </c>
+      <c r="I90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>116</v>
+      </c>
+      <c r="B91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C91" t="s">
+        <v>74</v>
+      </c>
+      <c r="D91" t="s">
+        <v>74</v>
+      </c>
+      <c r="I91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>116</v>
+      </c>
+      <c r="B92" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" t="s">
+        <v>78</v>
+      </c>
+      <c r="D92" t="s">
+        <v>78</v>
+      </c>
+      <c r="I92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" t="s">
+        <v>98</v>
+      </c>
+      <c r="D93" t="s">
+        <v>98</v>
+      </c>
+      <c r="I93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>116</v>
+      </c>
+      <c r="B94" t="s">
+        <v>66</v>
+      </c>
+      <c r="C94" t="s">
+        <v>100</v>
+      </c>
+      <c r="D94" t="s">
+        <v>100</v>
+      </c>
+      <c r="I94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>116</v>
+      </c>
+      <c r="B95" t="s">
+        <v>66</v>
+      </c>
+      <c r="C95" t="s">
+        <v>113</v>
+      </c>
+      <c r="D95" t="s">
+        <v>113</v>
+      </c>
+      <c r="I95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" t="s">
+        <v>66</v>
+      </c>
+      <c r="C96" t="s">
+        <v>86</v>
+      </c>
+      <c r="D96" t="s">
+        <v>86</v>
+      </c>
+      <c r="I96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B97" t="s">
+        <v>66</v>
+      </c>
+      <c r="C97" t="s">
+        <v>101</v>
+      </c>
+      <c r="D97" t="s">
+        <v>101</v>
+      </c>
+      <c r="I97">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>116</v>
+      </c>
+      <c r="B98" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" t="s">
+        <v>102</v>
+      </c>
+      <c r="D98" t="s">
+        <v>102</v>
+      </c>
+      <c r="I98">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>116</v>
+      </c>
+      <c r="B99" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" t="s">
+        <v>103</v>
+      </c>
+      <c r="D99" t="s">
+        <v>103</v>
+      </c>
+      <c r="I99">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="B100" t="s">
+        <v>66</v>
+      </c>
+      <c r="C100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>116</v>
+      </c>
+      <c r="B101" t="s">
+        <v>66</v>
+      </c>
+      <c r="C101" t="s">
+        <v>20</v>
+      </c>
+      <c r="D101" t="s">
+        <v>20</v>
+      </c>
+      <c r="I101">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102" t="s">
+        <v>67</v>
+      </c>
+      <c r="C102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" t="s">
+        <v>11</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103" t="s">
+        <v>67</v>
+      </c>
+      <c r="C103" t="s">
+        <v>71</v>
+      </c>
+      <c r="D103" t="s">
+        <v>71</v>
+      </c>
+      <c r="I103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>116</v>
+      </c>
+      <c r="B104" t="s">
+        <v>67</v>
+      </c>
+      <c r="C104" t="s">
+        <v>75</v>
+      </c>
+      <c r="D104" t="s">
+        <v>75</v>
+      </c>
+      <c r="I104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" t="s">
+        <v>67</v>
+      </c>
+      <c r="C105" t="s">
+        <v>37</v>
+      </c>
+      <c r="D105" t="s">
+        <v>37</v>
+      </c>
+      <c r="I105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>116</v>
+      </c>
+      <c r="B106" t="s">
+        <v>67</v>
+      </c>
+      <c r="C106" t="s">
+        <v>80</v>
+      </c>
+      <c r="D106" t="s">
+        <v>80</v>
+      </c>
+      <c r="I106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>116</v>
+      </c>
+      <c r="B107" t="s">
+        <v>67</v>
+      </c>
+      <c r="C107" t="s">
+        <v>83</v>
+      </c>
+      <c r="D107" t="s">
+        <v>83</v>
+      </c>
+      <c r="I107">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108" t="s">
+        <v>67</v>
+      </c>
+      <c r="C108" t="s">
+        <v>77</v>
+      </c>
+      <c r="D108" t="s">
+        <v>77</v>
+      </c>
+      <c r="I108">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>116</v>
+      </c>
+      <c r="B109" t="s">
+        <v>67</v>
+      </c>
+      <c r="C109" t="s">
+        <v>104</v>
+      </c>
+      <c r="D109" t="s">
+        <v>104</v>
+      </c>
+      <c r="I109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>116</v>
+      </c>
+      <c r="B110" t="s">
+        <v>67</v>
+      </c>
+      <c r="C110" t="s">
+        <v>105</v>
+      </c>
+      <c r="D110" t="s">
+        <v>105</v>
+      </c>
+      <c r="I110">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" t="s">
+        <v>67</v>
+      </c>
+      <c r="C111" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" t="s">
+        <v>114</v>
+      </c>
+      <c r="I111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>116</v>
+      </c>
+      <c r="B112" t="s">
+        <v>67</v>
+      </c>
+      <c r="C112" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112" t="s">
+        <v>74</v>
+      </c>
+      <c r="I112">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113" t="s">
+        <v>67</v>
+      </c>
+      <c r="C113" t="s">
+        <v>78</v>
+      </c>
+      <c r="D113" t="s">
+        <v>78</v>
+      </c>
+      <c r="I113">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" t="s">
+        <v>67</v>
+      </c>
+      <c r="C114" t="s">
+        <v>106</v>
+      </c>
+      <c r="D114" t="s">
+        <v>106</v>
+      </c>
+      <c r="I114">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>116</v>
+      </c>
+      <c r="B115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C115" t="s">
+        <v>107</v>
+      </c>
+      <c r="D115" t="s">
+        <v>107</v>
+      </c>
+      <c r="I115">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>67</v>
+      </c>
+      <c r="C116" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" t="s">
+        <v>18</v>
+      </c>
+      <c r="I116">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>67</v>
+      </c>
+      <c r="C117" t="s">
+        <v>20</v>
+      </c>
+      <c r="D117" t="s">
+        <v>20</v>
+      </c>
+      <c r="I117">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>68</v>
+      </c>
+      <c r="C118" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" t="s">
+        <v>11</v>
+      </c>
+      <c r="I118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>116</v>
+      </c>
+      <c r="B119" t="s">
+        <v>68</v>
+      </c>
+      <c r="C119" t="s">
+        <v>72</v>
+      </c>
+      <c r="D119" t="s">
+        <v>72</v>
+      </c>
+      <c r="I119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>116</v>
+      </c>
+      <c r="B120" t="s">
+        <v>68</v>
+      </c>
+      <c r="C120" t="s">
+        <v>74</v>
+      </c>
+      <c r="D120" t="s">
+        <v>74</v>
+      </c>
+      <c r="I120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>116</v>
+      </c>
+      <c r="B121" t="s">
+        <v>68</v>
+      </c>
+      <c r="C121" t="s">
+        <v>78</v>
+      </c>
+      <c r="D121" t="s">
+        <v>78</v>
+      </c>
+      <c r="I121">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>116</v>
+      </c>
+      <c r="B122" t="s">
+        <v>68</v>
+      </c>
+      <c r="C122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" t="s">
+        <v>18</v>
+      </c>
+      <c r="I122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>116</v>
+      </c>
+      <c r="B123" t="s">
+        <v>68</v>
+      </c>
+      <c r="C123" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123" t="s">
+        <v>20</v>
+      </c>
+      <c r="I123">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>116</v>
+      </c>
+      <c r="B124" t="s">
+        <v>69</v>
+      </c>
+      <c r="C124" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" t="s">
+        <v>11</v>
+      </c>
+      <c r="I124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>116</v>
+      </c>
+      <c r="B125" t="s">
+        <v>69</v>
+      </c>
+      <c r="C125" t="s">
+        <v>71</v>
+      </c>
+      <c r="D125" t="s">
+        <v>71</v>
+      </c>
+      <c r="I125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>116</v>
+      </c>
+      <c r="B126" t="s">
+        <v>69</v>
+      </c>
+      <c r="C126" t="s">
+        <v>76</v>
+      </c>
+      <c r="D126" t="s">
+        <v>76</v>
+      </c>
+      <c r="I126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>116</v>
+      </c>
+      <c r="B127" t="s">
+        <v>69</v>
+      </c>
+      <c r="C127" t="s">
+        <v>79</v>
+      </c>
+      <c r="D127" t="s">
+        <v>79</v>
+      </c>
+      <c r="I127">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>116</v>
+      </c>
+      <c r="B128" t="s">
+        <v>69</v>
+      </c>
+      <c r="C128" t="s">
+        <v>81</v>
+      </c>
+      <c r="D128" t="s">
+        <v>81</v>
+      </c>
+      <c r="I128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" t="s">
+        <v>69</v>
+      </c>
+      <c r="C129" t="s">
+        <v>77</v>
+      </c>
+      <c r="D129" t="s">
+        <v>77</v>
+      </c>
+      <c r="I129">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>116</v>
+      </c>
+      <c r="B130" t="s">
+        <v>69</v>
+      </c>
+      <c r="C130" t="s">
+        <v>108</v>
+      </c>
+      <c r="D130" t="s">
+        <v>108</v>
+      </c>
+      <c r="I130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>116</v>
+      </c>
+      <c r="B131" t="s">
+        <v>69</v>
+      </c>
+      <c r="C131" t="s">
+        <v>109</v>
+      </c>
+      <c r="D131" t="s">
+        <v>109</v>
+      </c>
+      <c r="I131">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>116</v>
+      </c>
+      <c r="B132" t="s">
+        <v>69</v>
+      </c>
+      <c r="C132" t="s">
+        <v>110</v>
+      </c>
+      <c r="D132" t="s">
+        <v>110</v>
+      </c>
+      <c r="I132">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>116</v>
+      </c>
+      <c r="B133" t="s">
+        <v>69</v>
+      </c>
+      <c r="C133" t="s">
+        <v>102</v>
+      </c>
+      <c r="D133" t="s">
+        <v>102</v>
+      </c>
+      <c r="I133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>116</v>
+      </c>
+      <c r="B134" t="s">
+        <v>69</v>
+      </c>
+      <c r="C134" t="s">
+        <v>18</v>
+      </c>
+      <c r="D134" t="s">
+        <v>18</v>
+      </c>
+      <c r="I134">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>116</v>
+      </c>
+      <c r="B135" t="s">
+        <v>69</v>
+      </c>
+      <c r="C135" t="s">
+        <v>20</v>
+      </c>
+      <c r="D135" t="s">
+        <v>20</v>
+      </c>
+      <c r="I135">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>116</v>
+      </c>
+      <c r="B136" t="s">
+        <v>70</v>
+      </c>
+      <c r="C136" t="s">
+        <v>11</v>
+      </c>
+      <c r="D136" t="s">
+        <v>11</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>116</v>
+      </c>
+      <c r="B137" t="s">
+        <v>70</v>
+      </c>
+      <c r="C137" t="s">
+        <v>95</v>
+      </c>
+      <c r="D137" t="s">
+        <v>95</v>
+      </c>
+      <c r="I137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>116</v>
+      </c>
+      <c r="B138" t="s">
+        <v>70</v>
+      </c>
+      <c r="C138" t="s">
+        <v>58</v>
+      </c>
+      <c r="D138" t="s">
+        <v>58</v>
+      </c>
+      <c r="I138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>116</v>
+      </c>
+      <c r="B139" t="s">
+        <v>70</v>
+      </c>
+      <c r="C139" t="s">
+        <v>74</v>
+      </c>
+      <c r="D139" t="s">
+        <v>74</v>
+      </c>
+      <c r="I139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>116</v>
+      </c>
+      <c r="B140" t="s">
+        <v>70</v>
+      </c>
+      <c r="C140" t="s">
+        <v>78</v>
+      </c>
+      <c r="D140" t="s">
+        <v>78</v>
+      </c>
+      <c r="I140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>116</v>
+      </c>
+      <c r="B141" t="s">
+        <v>70</v>
+      </c>
+      <c r="C141" t="s">
+        <v>18</v>
+      </c>
+      <c r="D141" t="s">
+        <v>18</v>
+      </c>
+      <c r="I141">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>116</v>
+      </c>
+      <c r="B142" t="s">
+        <v>70</v>
+      </c>
+      <c r="C142" t="s">
+        <v>20</v>
+      </c>
+      <c r="D142" t="s">
+        <v>20</v>
+      </c>
+      <c r="I142">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>116</v>
+      </c>
+      <c r="B143" t="s">
+        <v>95</v>
+      </c>
+      <c r="C143" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" t="s">
+        <v>11</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>116</v>
+      </c>
+      <c r="B144" t="s">
+        <v>95</v>
+      </c>
+      <c r="C144" t="s">
+        <v>72</v>
+      </c>
+      <c r="D144" t="s">
+        <v>72</v>
+      </c>
+      <c r="I144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>116</v>
+      </c>
+      <c r="B145" t="s">
+        <v>95</v>
+      </c>
+      <c r="C145" t="s">
+        <v>54</v>
+      </c>
+      <c r="D145" t="s">
+        <v>54</v>
+      </c>
+      <c r="I145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>116</v>
+      </c>
+      <c r="B146" t="s">
+        <v>95</v>
+      </c>
+      <c r="C146" t="s">
+        <v>18</v>
+      </c>
+      <c r="D146" t="s">
+        <v>18</v>
+      </c>
+      <c r="I146">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>116</v>
+      </c>
+      <c r="B147" t="s">
+        <v>95</v>
+      </c>
+      <c r="C147" t="s">
+        <v>20</v>
+      </c>
+      <c r="D147" t="s">
+        <v>20</v>
+      </c>
+      <c r="I147">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>